<commit_message>
Re-organized the HFC_CONTAINER & RECEIVING section
</commit_message>
<xml_diff>
--- a/ER DIAGRAM.xlsx
+++ b/ER DIAGRAM.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="202">
   <si>
     <t>SEASON</t>
   </si>
@@ -469,9 +469,6 @@
   </si>
   <si>
     <t>RECEIVING</t>
-  </si>
-  <si>
-    <t>REC_NBR</t>
   </si>
   <si>
     <t>REC_DATE</t>
@@ -548,9 +545,6 @@
     <t>BUY_GROUP_SUB</t>
   </si>
   <si>
-    <t>***CHALLENGE: HOW TO DEAL WITH RARE CASE WHEN A GREEN_BAR/STYLE/COLOR NEEDS TO GET ATTACHED TO MULTIPLE HFCS?</t>
-  </si>
-  <si>
     <t>SOURCE_BUY_MAKER_ECOM.csv'</t>
   </si>
   <si>
@@ -561,17 +555,64 @@
     <t>SOURCE_STYLE_MASTER_SLV_AND_SIZE.csv</t>
   </si>
   <si>
-    <t>SOURCE_CONTAINER_RECVD.xlsx</t>
-  </si>
-  <si>
     <t>SOURCE_CUSTOMER.csv</t>
   </si>
   <si>
     <t>SOURCE_SIZE_RANGE_MASTER.csv</t>
   </si>
   <si>
+    <t>***delete once truly received</t>
+  </si>
+  <si>
+    <t>RESERVE</t>
+  </si>
+  <si>
+    <t>decimal(10,2)</t>
+  </si>
+  <si>
+    <t>decimal(21,2)</t>
+  </si>
+  <si>
+    <t>DIFF</t>
+  </si>
+  <si>
+    <t>SHORT_OVER</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">60.11;
+      <t xml:space="preserve">10.40.44
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'000000' indicates a temp close-out order</t>
+    </r>
+  </si>
+  <si>
+    <t>HFC_2</t>
+  </si>
+  <si>
+    <t>manual add in special case*</t>
+  </si>
+  <si>
+    <t>***SPECIAL CASE: one GREEN_BAR/STYLE/COLOR attaches to multiple HFC's</t>
+  </si>
+  <si>
+    <t>CTN_TO_COME</t>
+  </si>
+  <si>
+    <t>INVOICE_NBR</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SOURCE_RECEIVING_NEW.xlsx
 </t>
     </r>
     <r>
@@ -582,27 +623,80 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CTRL_NBR = 1 is used to "fake" receiving***</t>
+      <t>1: FAKE***
+2: INV ADJ.</t>
     </r>
   </si>
   <si>
-    <t>***delete once truly received</t>
-  </si>
-  <si>
-    <t>RESERVE</t>
-  </si>
-  <si>
-    <t>decimal(10,2)</t>
-  </si>
-  <si>
-    <t>decimal(21,2)</t>
+    <t>SOURCE_RECEIVING_NEW.xlsx</t>
+  </si>
+  <si>
+    <t>REC_S1</t>
+  </si>
+  <si>
+    <t>REC_S2</t>
+  </si>
+  <si>
+    <t>REC_S3</t>
+  </si>
+  <si>
+    <t>REC_S4</t>
+  </si>
+  <si>
+    <t>REC_S5</t>
+  </si>
+  <si>
+    <t>REC_S6</t>
+  </si>
+  <si>
+    <t>REC_S7</t>
+  </si>
+  <si>
+    <t>REC_S8</t>
+  </si>
+  <si>
+    <t>***This table holds data different from 60.11 in that it takes inv adj. into consideration</t>
+  </si>
+  <si>
+    <r>
+      <t>auto-calculated
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>need SHORT_OVER table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>***ETA does not go with CONTAINER_NBR due to multiple "AIR" / "FEDEX"</t>
+  </si>
+  <si>
+    <t>SOURCE_SHORT-OVER.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,6 +753,32 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -757,7 +877,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -859,6 +979,29 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -868,6 +1011,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -876,9 +1022,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1165,8 +1308,8 @@
   </sheetPr>
   <dimension ref="B2:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1317,7 @@
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="3.7109375" customWidth="1"/>
     <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
@@ -1188,40 +1331,40 @@
     <col min="16" max="16" width="3.7109375" customWidth="1"/>
     <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.5703125" customWidth="1"/>
-    <col min="19" max="19" width="24.5703125" customWidth="1"/>
-    <col min="20" max="20" width="16.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.28515625" customWidth="1"/>
+    <col min="20" max="20" width="25.85546875" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
       <c r="E2" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52"/>
       <c r="J2" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
       <c r="O2" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="Q2" s="45" t="s">
+      <c r="Q2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
       <c r="T2" s="35" t="s">
         <v>112</v>
       </c>
@@ -1237,7 +1380,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>6</v>
@@ -1287,7 +1430,7 @@
         <v>53</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>32</v>
@@ -1323,15 +1466,15 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="B5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>33</v>
@@ -1365,15 +1508,15 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3"/>
       <c r="E6" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>0</v>
@@ -1408,14 +1551,14 @@
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="8" t="s">
-        <v>176</v>
+      <c r="E7" s="28" t="s">
+        <v>189</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>8</v>
@@ -1440,18 +1583,27 @@
         <v>118</v>
       </c>
       <c r="Q7" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R7" s="14" t="s">
         <v>3</v>
       </c>
       <c r="S7" s="14"/>
       <c r="T7" s="36" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="E8" s="10"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="43" t="s">
+        <v>199</v>
+      </c>
       <c r="G8" s="22" t="s">
         <v>48</v>
       </c>
@@ -1475,17 +1627,27 @@
         <v>118</v>
       </c>
       <c r="Q8" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R8" s="15" t="s">
         <v>3</v>
       </c>
       <c r="S8" s="15"/>
       <c r="T8" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="G9" s="22" t="s">
         <v>1</v>
       </c>
@@ -1500,32 +1662,30 @@
         <v>27</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N9" s="14"/>
       <c r="O9" s="16" t="s">
         <v>118</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R9" s="15" t="s">
         <v>3</v>
       </c>
       <c r="S9" s="15"/>
       <c r="T9" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="11" t="s">
-        <v>112</v>
-      </c>
+      <c r="B10" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" s="48"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="46"/>
       <c r="G10" s="21" t="s">
         <v>86</v>
       </c>
@@ -1540,36 +1700,28 @@
         <v>25</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N10" s="14"/>
       <c r="O10" s="16" t="s">
         <v>118</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R10" s="15" t="s">
         <v>3</v>
       </c>
       <c r="S10" s="15"/>
       <c r="T10" s="36" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>179</v>
-      </c>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="47"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="46"/>
       <c r="G11" s="22" t="s">
         <v>87</v>
       </c>
@@ -1584,36 +1736,24 @@
         <v>23</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="16" t="s">
         <v>118</v>
       </c>
       <c r="Q11" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R11" s="15" t="s">
         <v>3</v>
       </c>
       <c r="S11" s="15"/>
       <c r="T11" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="28">
-        <v>60.11</v>
-      </c>
       <c r="G12" s="22" t="s">
         <v>88</v>
       </c>
@@ -1635,28 +1775,24 @@
         <v>118</v>
       </c>
       <c r="Q12" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R12" s="15" t="s">
         <v>3</v>
       </c>
       <c r="S12" s="15"/>
       <c r="T12" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="28">
-        <v>60.11</v>
+      <c r="B13" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="51"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="G13" s="24" t="s">
         <v>94</v>
@@ -1666,7 +1802,7 @@
       </c>
       <c r="I13" s="24"/>
       <c r="J13" s="27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L13" s="14" t="s">
         <v>106</v>
@@ -1679,28 +1815,28 @@
         <v>118</v>
       </c>
       <c r="Q13" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R13" s="15" t="s">
         <v>3</v>
       </c>
       <c r="S13" s="15"/>
       <c r="T13" s="36" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="28">
-        <v>60.11</v>
+        <v>7</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>188</v>
       </c>
       <c r="G14" s="24" t="s">
         <v>115</v>
@@ -1725,26 +1861,28 @@
         <v>118</v>
       </c>
       <c r="Q14" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R14" s="15" t="s">
         <v>3</v>
       </c>
       <c r="S14" s="15"/>
       <c r="T14" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="C15" s="24" t="s">
+      <c r="B15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="28">
-        <v>60.11</v>
+      <c r="D15" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>189</v>
       </c>
       <c r="G15" s="24" t="s">
         <v>93</v>
@@ -1754,13 +1892,13 @@
       </c>
       <c r="I15" s="26"/>
       <c r="J15" s="27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L15" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="M15" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N15" s="14"/>
       <c r="O15" s="16" t="s">
@@ -1780,15 +1918,17 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="28">
-        <v>60.11</v>
+      <c r="B16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>189</v>
       </c>
       <c r="G16" s="24" t="s">
         <v>54</v>
@@ -1804,7 +1944,7 @@
         <v>109</v>
       </c>
       <c r="M16" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N16" s="14"/>
       <c r="O16" s="16" t="s">
@@ -1812,15 +1952,17 @@
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="28">
-        <v>60.11</v>
+      <c r="B17" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>189</v>
       </c>
       <c r="L17" s="14" t="s">
         <v>110</v>
@@ -1836,12 +1978,18 @@
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="40" t="s">
-        <v>180</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="B18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="L18" s="14" t="s">
         <v>15</v>
       </c>
@@ -1850,27 +1998,33 @@
       </c>
       <c r="N18" s="33"/>
       <c r="O18" s="16" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q18" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q18" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="R18" s="46"/>
-      <c r="S18" s="46"/>
+      <c r="R18" s="56"/>
+      <c r="S18" s="56"/>
       <c r="T18" s="35" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="2:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="G19" s="46" t="s">
+    <row r="19" spans="2:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="G19" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
       <c r="J19" s="35" t="s">
         <v>112</v>
       </c>
@@ -1882,7 +2036,7 @@
       </c>
       <c r="N19" s="33"/>
       <c r="O19" s="25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q19" s="17" t="s">
         <v>20</v>
@@ -1893,11 +2047,21 @@
       <c r="S19" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="T19" s="36" t="s">
-        <v>126</v>
+      <c r="T19" s="42" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="44"/>
+      <c r="E20" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="G20" s="2" t="s">
         <v>6</v>
       </c>
@@ -1918,7 +2082,7 @@
       </c>
       <c r="N20" s="33"/>
       <c r="O20" s="25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q20" s="17" t="s">
         <v>10</v>
@@ -1934,6 +2098,16 @@
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="44"/>
+      <c r="E21" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="G21" s="2" t="s">
         <v>10</v>
       </c>
@@ -1947,14 +2121,14 @@
         <v>117</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M21" s="15" t="s">
         <v>45</v>
       </c>
       <c r="N21" s="34"/>
       <c r="O21" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q21" s="17" t="s">
         <v>123</v>
@@ -1970,6 +2144,16 @@
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="44"/>
+      <c r="E22" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="G22" s="2" t="s">
         <v>11</v>
       </c>
@@ -1983,14 +2167,14 @@
         <v>117</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M22" s="15" t="s">
         <v>45</v>
       </c>
       <c r="N22" s="34"/>
       <c r="O22" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q22" s="15" t="s">
         <v>8</v>
@@ -2004,6 +2188,16 @@
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="44"/>
+      <c r="E23" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
@@ -2015,14 +2209,14 @@
         <v>117</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M23" s="24" t="s">
         <v>45</v>
       </c>
       <c r="N23" s="26"/>
       <c r="O23" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q23" s="15" t="s">
         <v>48</v>
@@ -2038,6 +2232,16 @@
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="44"/>
+      <c r="E24" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="G24" s="12" t="s">
         <v>13</v>
       </c>
@@ -2047,7 +2251,7 @@
       <c r="I24" s="12"/>
       <c r="J24" s="9"/>
       <c r="L24" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M24" s="24" t="s">
         <v>107</v>
@@ -2068,6 +2272,16 @@
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="44"/>
+      <c r="E25" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="G25" s="3" t="s">
         <v>114</v>
       </c>
@@ -2093,7 +2307,7 @@
         <v>119</v>
       </c>
       <c r="Q25" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R25" s="15" t="s">
         <v>2</v>
@@ -2104,6 +2318,16 @@
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="44"/>
+      <c r="E26" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="G26" s="3" t="s">
         <v>103</v>
       </c>
@@ -2119,7 +2343,7 @@
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="Q26" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R26" s="15" t="s">
         <v>2</v>
@@ -2130,11 +2354,21 @@
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="44"/>
+      <c r="E27" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="G27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="8" t="s">
@@ -2152,21 +2386,31 @@
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="44"/>
+      <c r="E28" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="G28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="L28" s="45" t="s">
+      <c r="L28" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
       <c r="O28" s="11" t="s">
         <v>112</v>
       </c>
@@ -2182,11 +2426,17 @@
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
       <c r="G29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="8" t="s">
@@ -2201,14 +2451,14 @@
       <c r="N29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O29" s="44" t="s">
-        <v>178</v>
+      <c r="O29" s="54" t="s">
+        <v>175</v>
       </c>
       <c r="Q29" s="15" t="s">
         <v>23</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="S29" s="15"/>
       <c r="T29" s="36" t="s">
@@ -2216,11 +2466,17 @@
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
       <c r="G30" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="8" t="s">
@@ -2235,7 +2491,7 @@
       <c r="N30" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O30" s="44"/>
+      <c r="O30" s="54"/>
       <c r="Q30" s="15" t="s">
         <v>28</v>
       </c>
@@ -2248,6 +2504,10 @@
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="45"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
       <c r="G31" s="1" t="s">
         <v>56</v>
       </c>
@@ -2267,12 +2527,12 @@
       <c r="N31" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O31" s="44"/>
+      <c r="O31" s="54"/>
       <c r="Q31" s="15" t="s">
         <v>127</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="S31" s="15"/>
       <c r="T31" s="36" t="s">
@@ -2299,7 +2559,7 @@
       <c r="N32" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O32" s="44"/>
+      <c r="O32" s="54"/>
       <c r="Q32" s="15" t="s">
         <v>29</v>
       </c>
@@ -2311,7 +2571,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" s="51"/>
+      <c r="D33" s="52"/>
       <c r="G33" s="1" t="s">
         <v>58</v>
       </c>
@@ -2331,19 +2596,31 @@
       <c r="N33" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O33" s="44"/>
+      <c r="O33" s="54"/>
       <c r="Q33" s="15" t="s">
         <v>129</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="S33" s="15"/>
       <c r="T33" s="36" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>201</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>59</v>
       </c>
@@ -2363,7 +2640,7 @@
       <c r="N34" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O34" s="44"/>
+      <c r="O34" s="54"/>
       <c r="Q34" s="15" t="s">
         <v>30</v>
       </c>
@@ -2375,7 +2652,19 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>201</v>
+      </c>
       <c r="G35" s="1" t="s">
         <v>60</v>
       </c>
@@ -2395,7 +2684,7 @@
       <c r="N35" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O35" s="44"/>
+      <c r="O35" s="54"/>
       <c r="Q35" s="15" t="s">
         <v>31</v>
       </c>
@@ -2407,7 +2696,19 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>201</v>
+      </c>
       <c r="G36" s="1" t="s">
         <v>61</v>
       </c>
@@ -2427,7 +2728,7 @@
       <c r="N36" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O36" s="44"/>
+      <c r="O36" s="54"/>
       <c r="Q36" s="15" t="s">
         <v>36</v>
       </c>
@@ -2439,7 +2740,17 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="14"/>
+      <c r="E37" s="41" t="s">
+        <v>201</v>
+      </c>
       <c r="G37" s="1" t="s">
         <v>62</v>
       </c>
@@ -2459,7 +2770,7 @@
       <c r="N37" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="O37" s="44"/>
+      <c r="O37" s="54"/>
       <c r="Q37" s="15" t="s">
         <v>37</v>
       </c>
@@ -2471,7 +2782,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="7:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20" ht="45" x14ac:dyDescent="0.25">
       <c r="G38" s="1" t="s">
         <v>63</v>
       </c>
@@ -2489,13 +2800,13 @@
         <v>42</v>
       </c>
       <c r="S38" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T38" s="37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G39" s="1" t="s">
         <v>65</v>
       </c>
@@ -2507,24 +2818,24 @@
         <v>117</v>
       </c>
       <c r="Q39" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R39" s="31" t="s">
         <v>42</v>
       </c>
       <c r="S39" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T39" s="37" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G40" s="1" t="s">
         <v>66</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="8" t="s">
@@ -2543,12 +2854,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G41" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I41" s="1"/>
       <c r="J41" s="8" t="s">
@@ -2565,12 +2876,12 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G42" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="8" t="s">
@@ -2587,12 +2898,12 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G43" s="1" t="s">
         <v>69</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="8" t="s">
@@ -2609,7 +2920,7 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="44" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G44" s="24" t="s">
         <v>54</v>
       </c>
@@ -2631,7 +2942,7 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q45" s="15" t="s">
         <v>134</v>
       </c>
@@ -2643,7 +2954,7 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q46" s="15" t="s">
         <v>135</v>
       </c>
@@ -2655,12 +2966,12 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="47" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G47" s="45" t="s">
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G47" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="55"/>
       <c r="J47" s="11" t="s">
         <v>112</v>
       </c>
@@ -2675,7 +2986,7 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="48" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="G48" s="2" t="s">
         <v>48</v>
       </c>
@@ -2685,8 +2996,8 @@
       <c r="I48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J48" s="44" t="s">
-        <v>177</v>
+      <c r="J48" s="54" t="s">
+        <v>174</v>
       </c>
       <c r="Q48" s="15" t="s">
         <v>137</v>
@@ -2707,7 +3018,7 @@
         <v>46</v>
       </c>
       <c r="I49" s="1"/>
-      <c r="J49" s="44"/>
+      <c r="J49" s="54"/>
       <c r="Q49" s="14" t="s">
         <v>138</v>
       </c>
@@ -2732,11 +3043,11 @@
       </c>
     </row>
     <row r="51" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G51" s="45" t="s">
+      <c r="G51" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="H51" s="45"/>
-      <c r="I51" s="45"/>
+      <c r="H51" s="55"/>
+      <c r="I51" s="55"/>
       <c r="J51" s="11" t="s">
         <v>112</v>
       </c>
@@ -2761,7 +3072,7 @@
       <c r="I52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J52" s="44" t="s">
+      <c r="J52" s="54" t="s">
         <v>120</v>
       </c>
       <c r="Q52" s="15" t="s">
@@ -2785,7 +3096,7 @@
       <c r="I53" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J53" s="44"/>
+      <c r="J53" s="54"/>
       <c r="Q53" s="15" t="s">
         <v>142</v>
       </c>
@@ -2807,7 +3118,7 @@
       <c r="I54" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J54" s="44"/>
+      <c r="J54" s="54"/>
       <c r="Q54" s="15" t="s">
         <v>143</v>
       </c>
@@ -2829,7 +3140,7 @@
       <c r="I55" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J55" s="44"/>
+      <c r="J55" s="54"/>
       <c r="Q55" s="15" t="s">
         <v>144</v>
       </c>
@@ -2851,7 +3162,7 @@
       <c r="I56" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J56" s="44"/>
+      <c r="J56" s="54"/>
       <c r="Q56" s="15" t="s">
         <v>145</v>
       </c>
@@ -2873,7 +3184,7 @@
       <c r="I57" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J57" s="44"/>
+      <c r="J57" s="54"/>
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
       <c r="S57" s="4"/>
@@ -2888,7 +3199,7 @@
       <c r="I58" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="44"/>
+      <c r="J58" s="54"/>
     </row>
     <row r="59" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G59" s="7" t="s">
@@ -2900,12 +3211,12 @@
       <c r="I59" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="44"/>
-      <c r="Q59" s="45" t="s">
+      <c r="J59" s="54"/>
+      <c r="Q59" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="R59" s="45"/>
-      <c r="S59" s="45"/>
+      <c r="R59" s="55"/>
+      <c r="S59" s="55"/>
       <c r="T59" s="35" t="s">
         <v>112</v>
       </c>
@@ -2920,7 +3231,7 @@
       <c r="I60" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J60" s="44"/>
+      <c r="J60" s="54"/>
       <c r="Q60" s="2" t="s">
         <v>20</v>
       </c>
@@ -2944,7 +3255,7 @@
       <c r="I61" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J61" s="44"/>
+      <c r="J61" s="54"/>
       <c r="Q61" s="2" t="s">
         <v>10</v>
       </c>
@@ -2968,7 +3279,7 @@
       <c r="I62" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J62" s="44"/>
+      <c r="J62" s="54"/>
       <c r="Q62" s="2" t="s">
         <v>123</v>
       </c>
@@ -2992,7 +3303,7 @@
       <c r="I63" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J63" s="44"/>
+      <c r="J63" s="54"/>
       <c r="Q63" s="5" t="s">
         <v>124</v>
       </c>
@@ -3014,7 +3325,7 @@
       <c r="I64" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J64" s="44"/>
+      <c r="J64" s="54"/>
       <c r="Q64" s="1" t="s">
         <v>0</v>
       </c>
@@ -3023,7 +3334,7 @@
       </c>
       <c r="S64" s="1"/>
       <c r="T64" s="38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="7:20" x14ac:dyDescent="0.25">
@@ -3036,7 +3347,7 @@
       <c r="I65" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J65" s="44"/>
+      <c r="J65" s="54"/>
       <c r="Q65" s="1" t="s">
         <v>54</v>
       </c>
@@ -3060,7 +3371,17 @@
       <c r="I66" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J66" s="44"/>
+      <c r="J66" s="54"/>
+      <c r="Q66" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="R66" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="S66" s="5"/>
+      <c r="T66" s="38" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="67" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G67" s="7" t="s">
@@ -3072,9 +3393,9 @@
       <c r="I67" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J67" s="44"/>
-    </row>
-    <row r="68" spans="7:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J67" s="54"/>
+    </row>
+    <row r="68" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G68" s="7" t="s">
         <v>62</v>
       </c>
@@ -3084,13 +3405,13 @@
       <c r="I68" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J68" s="44"/>
-      <c r="Q68" s="47" t="s">
-        <v>172</v>
-      </c>
-      <c r="R68" s="47"/>
-      <c r="S68" s="47"/>
-      <c r="T68" s="47"/>
+      <c r="J68" s="54"/>
+      <c r="Q68" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="R68" s="53"/>
+      <c r="S68" s="53"/>
+      <c r="T68" s="53"/>
     </row>
     <row r="69" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G69" s="7" t="s">
@@ -3102,12 +3423,14 @@
       <c r="I69" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J69" s="44"/>
+      <c r="J69" s="54"/>
+      <c r="Q69" s="49"/>
+      <c r="R69" s="49"/>
+      <c r="S69" s="49"/>
+      <c r="T69" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="J52:J69"/>
+  <mergeCells count="17">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="G51:I51"/>
     <mergeCell ref="Q2:S2"/>
@@ -3119,10 +3442,14 @@
     <mergeCell ref="L28:N28"/>
     <mergeCell ref="J48:J49"/>
     <mergeCell ref="O29:O37"/>
+    <mergeCell ref="Q69:T69"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="Q68:T68"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="J52:J69"/>
     <mergeCell ref="Q59:S59"/>
-    <mergeCell ref="Q68:T68"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
-  <pageSetup paperSize="17" scale="65" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="17" scale="58" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>